<commit_message>
Add early implementation of Edit, change Create
</commit_message>
<xml_diff>
--- a/projekt.xlsx
+++ b/projekt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\FinanceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF767E9A-409D-4085-B43D-24C4F369C5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B7AD32-A0E0-4AB8-9CE5-BFD3FB8574E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45F55355-C5E5-4E31-A492-D06A40B57353}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Tlo ogolne</t>
   </si>
@@ -89,6 +89,263 @@
     </r>
   </si>
   <si>
+    <t>BarChartViewModel (collection):
+int credits
+int charges</t>
+  </si>
+  <si>
+    <t>PieChartViewModel (collection):
+string name
+int value</t>
+  </si>
+  <si>
+    <t>SelectList Months</t>
+  </si>
+  <si>
+    <t>YearlySummaryViewModel:
+int balance
+int credits
+int charges</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OtherExpensesViewModel (collection):
+int id
+string name
+int value
+datetime date
+bool paid
+List, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Edit, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF4B76"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delete</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1ED88D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Paid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OverduePaymentsViewModel (collection):
+int id
+string name
+int value
+datetime date
+bool paid
+List, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Edit, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF4B76"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delete</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF1ED88D"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Paid</t>
+    </r>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Delete/Low</t>
+  </si>
+  <si>
+    <t>Create/High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(153, 102, 255, 1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(75, 192, 192, 1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(54, 162, 235, 1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(255, 99, 132, 1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(255, 159, 64, 1) </t>
+  </si>
+  <si>
+    <t>#FFDD33</t>
+  </si>
+  <si>
+    <t>Żółty</t>
+  </si>
+  <si>
+    <t>rgba(255, 221, 51, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(24,23,54,1) </t>
+  </si>
+  <si>
+    <t>rgba(56,53,96,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rgba(255,99,136) </t>
+  </si>
+  <si>
+    <t>rgba(62,220,195,1)</t>
+  </si>
+  <si>
+    <t>#3EDCC3</t>
+  </si>
+  <si>
+    <t>Intensywny zielony</t>
+  </si>
+  <si>
+    <t>Kolory do wykresów</t>
+  </si>
+  <si>
+    <t>RGBA:</t>
+  </si>
+  <si>
+    <t>HASH:</t>
+  </si>
+  <si>
+    <t>KOLOR:</t>
+  </si>
+  <si>
+    <t>Czerwony/Rozowy</t>
+  </si>
+  <si>
+    <t>Fioletowy</t>
+  </si>
+  <si>
+    <t>Ciemny fioletowy</t>
+  </si>
+  <si>
+    <t>Niebieski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#FF9F40 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#FF6384 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#36A2EB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#4BC0C0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#9966FF </t>
+  </si>
+  <si>
+    <t>Turkusowy</t>
+  </si>
+  <si>
+    <t>Fiolet</t>
+  </si>
+  <si>
+    <t>Różowy</t>
+  </si>
+  <si>
+    <t>Pomarańczowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#FF6388 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#383560 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">#181736 </t>
+  </si>
+  <si>
+    <t>OPIS:</t>
+  </si>
+  <si>
+    <t>Kroki implementacji:</t>
+  </si>
+  <si>
+    <t>1. Implementacja kolekcji</t>
+  </si>
+  <si>
+    <t>2. Implementacja podsumowań</t>
+  </si>
+  <si>
+    <t>3. Implementacja wykresów</t>
+  </si>
+  <si>
+    <t>4. Implementacja Create (Salary, Other, Ongoing)</t>
+  </si>
+  <si>
+    <t>5. Implementacja Delete (Salary, Other, Ongoing)</t>
+  </si>
+  <si>
+    <t>6. Implementacja Paid (Salary, Other, Ongoing)</t>
+  </si>
+  <si>
+    <t>7. Implementacja Edit (Salary, Other, Ongoing)</t>
+  </si>
+  <si>
+    <t>8. Frontend polish</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">OngoingExpensesViewModel (collection):
 int id
@@ -134,276 +391,19 @@
       </rPr>
       <t>, Paid</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+  </si>
+  <si>
+    <t xml:space="preserve">MonthlySummaryViewModel:
+int balanceOverall
+int creditsOverall
+int chargesOverall
+int balancePaid
+int creditsPaid
+int chargesPaid
 </t>
-    </r>
-  </si>
-  <si>
-    <t>BarChartViewModel (collection):
-int credits
-int charges</t>
-  </si>
-  <si>
-    <t>PieChartViewModel (collection):
-string name
-int value</t>
-  </si>
-  <si>
-    <t>SelectList Months</t>
-  </si>
-  <si>
-    <t>SalaryCreate</t>
-  </si>
-  <si>
-    <t>MonthlySummaryViewModel:
-int balance
-int credits
-int charges</t>
-  </si>
-  <si>
-    <t>YearlySummaryViewModel:
-int balance
-int credits
-int charges</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">OtherExpensesViewModel (collection):
-int id
-string name
-int value
-datetime date
-bool paid
-List, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Edit, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF4B76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delete</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF1ED88D"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Paid</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">OverduePaymentsViewModel (collection):
-int id
-string name
-int value
-datetime date
-bool paid
-List, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Edit, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF4B76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Delete</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF1ED88D"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Paid</t>
-    </r>
-  </si>
-  <si>
-    <t>Edit</t>
-  </si>
-  <si>
-    <t>Delete/Low</t>
-  </si>
-  <si>
-    <t>Create/High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(153, 102, 255, 1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(75, 192, 192, 1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(54, 162, 235, 1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(255, 99, 132, 1) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(255, 159, 64, 1) </t>
-  </si>
-  <si>
-    <t>#FFDD33</t>
-  </si>
-  <si>
-    <t>Żółty</t>
-  </si>
-  <si>
-    <t>rgba(255, 221, 51, 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(24,23,54,1) </t>
-  </si>
-  <si>
-    <t>rgba(56,53,96,1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rgba(255,99,136) </t>
-  </si>
-  <si>
-    <t>rgba(62,220,195,1)</t>
-  </si>
-  <si>
-    <t>#3EDCC3</t>
-  </si>
-  <si>
-    <t>Intensywny zielony</t>
-  </si>
-  <si>
-    <t>Kolory do wykresów</t>
-  </si>
-  <si>
-    <t>RGBA:</t>
-  </si>
-  <si>
-    <t>HASH:</t>
-  </si>
-  <si>
-    <t>KOLOR:</t>
-  </si>
-  <si>
-    <t>Czerwony/Rozowy</t>
-  </si>
-  <si>
-    <t>Fioletowy</t>
-  </si>
-  <si>
-    <t>Ciemny fioletowy</t>
-  </si>
-  <si>
-    <t>Niebieski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#FF9F40 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#FF6384 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#36A2EB </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#4BC0C0 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#9966FF </t>
-  </si>
-  <si>
-    <t>Turkusowy</t>
-  </si>
-  <si>
-    <t>Fiolet</t>
-  </si>
-  <si>
-    <t>Różowy</t>
-  </si>
-  <si>
-    <t>Pomarańczowy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#FF6388 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#383560 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">#181736 </t>
-  </si>
-  <si>
-    <t>OPIS:</t>
-  </si>
-  <si>
-    <t>Kroki implementacji:</t>
-  </si>
-  <si>
-    <t>1. Implementacja kolekcji</t>
-  </si>
-  <si>
-    <t>2. Implementacja operacji CRUD</t>
-  </si>
-  <si>
-    <t>3. Implementacja podsumowań</t>
-  </si>
-  <si>
-    <t>4. Implementacja wykresów</t>
-  </si>
-  <si>
-    <t>5. Frontend polish</t>
-  </si>
-  <si>
-    <t>ExpenseCreate</t>
+  </si>
+  <si>
+    <t>Savings Yearly Goal</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -663,6 +663,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -720,8 +723,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1053,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C74BCB17-4539-473B-93DD-0FD1B44EED04}">
   <dimension ref="A1:AQ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC27" sqref="AC27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,44 +1237,44 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="17"/>
+      <c r="D5" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="27"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z5" s="34"/>
-      <c r="AA5" s="34"/>
-      <c r="AB5" s="34"/>
-      <c r="AC5" s="34"/>
-      <c r="AD5" s="34"/>
-      <c r="AE5" s="34"/>
+      <c r="Y5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="15"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -1286,40 +1292,40 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="19"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="20"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="29"/>
+      <c r="W6" s="30"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
@@ -1339,35 +1345,35 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="20"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="33"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
@@ -1386,41 +1392,43 @@
       <c r="AP7" s="1"/>
       <c r="AQ7" s="1"/>
     </row>
-    <row r="8" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="20"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
@@ -1443,35 +1451,35 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="18"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="19"/>
-      <c r="W9" s="20"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="35"/>
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
@@ -1494,35 +1502,35 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="20"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="35"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="35"/>
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
@@ -1541,41 +1549,39 @@
       <c r="AP10" s="1"/>
       <c r="AQ10" s="1"/>
     </row>
-    <row r="11" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="18"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="19"/>
-      <c r="W11" s="20"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="35"/>
+      <c r="P11" s="35"/>
+      <c r="Q11" s="35"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
@@ -1598,35 +1604,35 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="19"/>
-      <c r="V12" s="19"/>
-      <c r="W12" s="20"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
@@ -1645,30 +1651,30 @@
       <c r="AP12" s="1"/>
       <c r="AQ12" s="1"/>
     </row>
-    <row r="13" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="19"/>
-      <c r="V13" s="19"/>
-      <c r="W13" s="20"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
@@ -1694,36 +1700,36 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="18"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="20"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z14" s="34"/>
-      <c r="AA14" s="34"/>
-      <c r="AB14" s="34"/>
-      <c r="AC14" s="34"/>
-      <c r="AD14" s="34"/>
-      <c r="AE14" s="34"/>
+      <c r="Y14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="15"/>
+      <c r="AB14" s="15"/>
+      <c r="AC14" s="15"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="15"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
@@ -1741,40 +1747,40 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="20"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
       <c r="AD15" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
@@ -1794,35 +1800,35 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="21"/>
-      <c r="T16" s="22"/>
-      <c r="U16" s="22"/>
-      <c r="V16" s="22"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
       <c r="W16" s="23"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Z16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
@@ -1847,41 +1853,43 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="18"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Z17" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
@@ -1906,40 +1914,40 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="19"/>
-      <c r="W18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="21"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Z18" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AE18" s="5"/>
       <c r="AF18" s="1"/>
@@ -1959,40 +1967,40 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="20"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="21"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Z19" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AE19" s="6"/>
       <c r="AF19" s="1"/>
@@ -2012,40 +2020,40 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="20"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="20"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="21"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AE20" s="7"/>
       <c r="AF20" s="1"/>
@@ -2061,30 +2069,30 @@
       <c r="AP20" s="1"/>
       <c r="AQ20" s="1"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="18"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="19"/>
-      <c r="W21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="21"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
@@ -2110,29 +2118,29 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="19"/>
-      <c r="W22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="21"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
@@ -2157,29 +2165,29 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="20"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="21"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Z23" s="13"/>
       <c r="AA23" s="13"/>
@@ -2204,29 +2212,29 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="19"/>
-      <c r="W24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="21"/>
       <c r="X24" s="1"/>
-      <c r="Y24" s="13" t="s">
-        <v>52</v>
+      <c r="Y24" s="14" t="s">
+        <v>49</v>
       </c>
       <c r="Z24" s="13"/>
       <c r="AA24" s="13"/>
@@ -2251,29 +2259,29 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="19"/>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="19"/>
-      <c r="W25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="21"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="Z25" s="13"/>
       <c r="AA25" s="13"/>
@@ -2298,29 +2306,29 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="19"/>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="19"/>
-      <c r="W26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="21"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Z26" s="13"/>
       <c r="AA26" s="13"/>
@@ -2345,29 +2353,29 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="18"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="19"/>
-      <c r="W27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="21"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Z27" s="13"/>
       <c r="AA27" s="13"/>
@@ -2392,28 +2400,30 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="21"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
-      <c r="W28" s="23"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="24"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="23"/>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23"/>
+      <c r="W28" s="24"/>
       <c r="X28" s="1"/>
-      <c r="Y28" s="13"/>
+      <c r="Y28" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="Z28" s="13"/>
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
@@ -2437,32 +2447,32 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="17"/>
+      <c r="D29" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="35"/>
+      <c r="T29" s="35"/>
+      <c r="U29" s="35"/>
+      <c r="V29" s="35"/>
+      <c r="W29" s="21"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="13"/>
+      <c r="Y29" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="Z29" s="13"/>
       <c r="AA29" s="13"/>
       <c r="AB29" s="13"/>
@@ -2486,28 +2496,30 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="20"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+      <c r="P30" s="35"/>
+      <c r="Q30" s="35"/>
+      <c r="R30" s="35"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="35"/>
+      <c r="U30" s="35"/>
+      <c r="V30" s="35"/>
+      <c r="W30" s="21"/>
       <c r="X30" s="1"/>
-      <c r="Y30" s="13"/>
+      <c r="Y30" s="13" t="s">
+        <v>55</v>
+      </c>
       <c r="Z30" s="13"/>
       <c r="AA30" s="13"/>
       <c r="AB30" s="13"/>
@@ -2531,26 +2543,26 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="19"/>
-      <c r="U31" s="19"/>
-      <c r="V31" s="19"/>
-      <c r="W31" s="20"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
+      <c r="V31" s="35"/>
+      <c r="W31" s="21"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
@@ -2576,26 +2588,26 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="19"/>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
-      <c r="S32" s="19"/>
-      <c r="T32" s="19"/>
-      <c r="U32" s="19"/>
-      <c r="V32" s="19"/>
-      <c r="W32" s="20"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+      <c r="P32" s="35"/>
+      <c r="Q32" s="35"/>
+      <c r="R32" s="35"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="35"/>
+      <c r="U32" s="35"/>
+      <c r="V32" s="35"/>
+      <c r="W32" s="21"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="13"/>
       <c r="Z32" s="13"/>
@@ -2621,26 +2633,26 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
-      <c r="S33" s="19"/>
-      <c r="T33" s="19"/>
-      <c r="U33" s="19"/>
-      <c r="V33" s="19"/>
-      <c r="W33" s="20"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="21"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
@@ -2666,26 +2678,26 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="20"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="35"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="21"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="13"/>
       <c r="Z34" s="13"/>
@@ -2711,26 +2723,26 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
-      <c r="P35" s="19"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="20"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="35"/>
+      <c r="U35" s="35"/>
+      <c r="V35" s="35"/>
+      <c r="W35" s="21"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
@@ -2756,26 +2768,26 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-      <c r="W36" s="20"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+      <c r="P36" s="35"/>
+      <c r="Q36" s="35"/>
+      <c r="R36" s="35"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="35"/>
+      <c r="U36" s="35"/>
+      <c r="V36" s="35"/>
+      <c r="W36" s="21"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="13"/>
       <c r="Z36" s="13"/>
@@ -2801,26 +2813,26 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19"/>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19"/>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
-      <c r="W37" s="20"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="35"/>
+      <c r="U37" s="35"/>
+      <c r="V37" s="35"/>
+      <c r="W37" s="21"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="13"/>
       <c r="Z37" s="13"/>
@@ -2846,26 +2858,26 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="18"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
-      <c r="S38" s="19"/>
-      <c r="T38" s="19"/>
-      <c r="U38" s="19"/>
-      <c r="V38" s="19"/>
-      <c r="W38" s="20"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+      <c r="P38" s="35"/>
+      <c r="Q38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="35"/>
+      <c r="U38" s="35"/>
+      <c r="V38" s="35"/>
+      <c r="W38" s="21"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="13"/>
       <c r="Z38" s="13"/>
@@ -2891,26 +2903,26 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
-      <c r="S39" s="19"/>
-      <c r="T39" s="19"/>
-      <c r="U39" s="19"/>
-      <c r="V39" s="19"/>
-      <c r="W39" s="20"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="35"/>
+      <c r="U39" s="35"/>
+      <c r="V39" s="35"/>
+      <c r="W39" s="21"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="13"/>
       <c r="Z39" s="13"/>
@@ -2932,30 +2944,30 @@
       <c r="AP39" s="1"/>
       <c r="AQ39" s="1"/>
     </row>
-    <row r="40" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="22"/>
-      <c r="Q40" s="22"/>
-      <c r="R40" s="22"/>
-      <c r="S40" s="22"/>
-      <c r="T40" s="22"/>
-      <c r="U40" s="22"/>
-      <c r="V40" s="22"/>
-      <c r="W40" s="23"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+      <c r="P40" s="35"/>
+      <c r="Q40" s="35"/>
+      <c r="R40" s="35"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="35"/>
+      <c r="U40" s="35"/>
+      <c r="V40" s="35"/>
+      <c r="W40" s="21"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
@@ -3137,11 +3149,11 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="13"/>
+      <c r="AC44" s="13"/>
       <c r="AD44" s="1"/>
       <c r="AE44" s="1"/>
       <c r="AF44" s="1"/>
@@ -3182,11 +3194,11 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="1"/>
-      <c r="AA45" s="1"/>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="1"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="13"/>
       <c r="AD45" s="1"/>
       <c r="AE45" s="1"/>
       <c r="AF45" s="1"/>
@@ -3202,7 +3214,7 @@
       <c r="AP45" s="1"/>
       <c r="AQ45" s="1"/>
     </row>
-    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3221,17 +3233,17 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="1"/>
-      <c r="AA46" s="1"/>
-      <c r="AB46" s="1"/>
-      <c r="AC46" s="1"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="13"/>
       <c r="AD46" s="1"/>
       <c r="AE46" s="1"/>
       <c r="AF46" s="1"/>
@@ -3257,26 +3269,21 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-      <c r="AA47" s="1"/>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AC47" s="13"/>
       <c r="AD47" s="1"/>
       <c r="AE47" s="1"/>
       <c r="AF47" s="1"/>
@@ -3302,26 +3309,21 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
-      <c r="Y48" s="1"/>
-      <c r="Z48" s="1"/>
-      <c r="AA48" s="1"/>
-      <c r="AB48" s="1"/>
-      <c r="AC48" s="1"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="13"/>
       <c r="AD48" s="1"/>
       <c r="AE48" s="1"/>
       <c r="AF48" s="1"/>
@@ -3347,26 +3349,21 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="1"/>
-      <c r="AA49" s="1"/>
-      <c r="AB49" s="1"/>
-      <c r="AC49" s="1"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
       <c r="AD49" s="1"/>
       <c r="AE49" s="1"/>
       <c r="AF49" s="1"/>
@@ -3392,26 +3389,21 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="1"/>
-      <c r="AA50" s="1"/>
-      <c r="AB50" s="1"/>
-      <c r="AC50" s="1"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="13"/>
       <c r="AD50" s="1"/>
       <c r="AE50" s="1"/>
       <c r="AF50" s="1"/>
@@ -3437,26 +3429,21 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
+      <c r="S51" s="13"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="1"/>
-      <c r="AA51" s="1"/>
-      <c r="AB51" s="1"/>
-      <c r="AC51" s="1"/>
+      <c r="Y51" s="13"/>
+      <c r="Z51" s="13"/>
+      <c r="AA51" s="13"/>
+      <c r="AB51" s="13"/>
+      <c r="AC51" s="13"/>
       <c r="AD51" s="1"/>
       <c r="AE51" s="1"/>
       <c r="AF51" s="1"/>
@@ -3482,26 +3469,21 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
+      <c r="S52" s="13"/>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13"/>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
+      <c r="Y52" s="13"/>
+      <c r="Z52" s="13"/>
+      <c r="AA52" s="13"/>
+      <c r="AB52" s="13"/>
+      <c r="AC52" s="13"/>
       <c r="AD52" s="1"/>
       <c r="AE52" s="1"/>
       <c r="AF52" s="1"/>
@@ -3527,26 +3509,21 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
+      <c r="S53" s="13"/>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13"/>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
-      <c r="Y53" s="1"/>
-      <c r="Z53" s="1"/>
-      <c r="AA53" s="1"/>
-      <c r="AB53" s="1"/>
-      <c r="AC53" s="1"/>
+      <c r="Y53" s="13"/>
+      <c r="Z53" s="13"/>
+      <c r="AA53" s="13"/>
+      <c r="AB53" s="13"/>
+      <c r="AC53" s="13"/>
       <c r="AD53" s="1"/>
       <c r="AE53" s="1"/>
       <c r="AF53" s="1"/>
@@ -3572,11 +3549,6 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
@@ -3608,21 +3580,20 @@
       <c r="AQ54" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
+    <mergeCell ref="D5:H16"/>
+    <mergeCell ref="I5:M16"/>
+    <mergeCell ref="D17:H28"/>
+    <mergeCell ref="S5:W7"/>
+    <mergeCell ref="D29:W40"/>
+    <mergeCell ref="I17:M28"/>
     <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="Y14:AE14"/>
-    <mergeCell ref="S5:W16"/>
+    <mergeCell ref="N17:R28"/>
     <mergeCell ref="S17:W28"/>
-    <mergeCell ref="N5:R28"/>
-    <mergeCell ref="I17:M28"/>
-    <mergeCell ref="I29:W40"/>
-    <mergeCell ref="D17:H28"/>
-    <mergeCell ref="D29:H40"/>
-    <mergeCell ref="I5:M16"/>
-    <mergeCell ref="D5:H7"/>
-    <mergeCell ref="D8:H10"/>
-    <mergeCell ref="D11:H13"/>
-    <mergeCell ref="D14:H16"/>
+    <mergeCell ref="N5:R7"/>
+    <mergeCell ref="N8:R16"/>
+    <mergeCell ref="S8:W16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add fully functional CRUD operations
</commit_message>
<xml_diff>
--- a/projekt.xlsx
+++ b/projekt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jedrulcia\Desktop\Jedrzej\Programowanko\github\FinanceTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B7AD32-A0E0-4AB8-9CE5-BFD3FB8574E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7072E37-D7FE-44A1-A3B3-2EE9166BCBC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45F55355-C5E5-4E31-A492-D06A40B57353}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45F55355-C5E5-4E31-A492-D06A40B57353}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -663,8 +663,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -693,41 +717,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1060,7 +1054,7 @@
   <dimension ref="A1:AQ54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC27" sqref="AC27"/>
+      <selection activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,44 +1231,44 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="16" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="25" t="s">
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="34" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="27"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="17"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="15" t="s">
+      <c r="Y5" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
@@ -1292,26 +1286,26 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="29"/>
-      <c r="U6" s="29"/>
-      <c r="V6" s="29"/>
-      <c r="W6" s="30"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="20"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="2" t="s">
         <v>27</v>
@@ -1345,26 +1339,26 @@
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="31"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="32"/>
-      <c r="V7" s="32"/>
-      <c r="W7" s="33"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="23"/>
       <c r="X7" s="1"/>
       <c r="Y7" s="2" t="s">
         <v>12</v>
@@ -1396,30 +1390,30 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="16" t="s">
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="16" t="s">
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="2" t="s">
         <v>13</v>
@@ -1451,26 +1445,26 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="21"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="2" t="s">
         <v>14</v>
@@ -1502,26 +1496,26 @@
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
       <c r="X10" s="1"/>
       <c r="Y10" s="2" t="s">
         <v>15</v>
@@ -1553,26 +1547,26 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="19"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
       <c r="X11" s="1"/>
       <c r="Y11" s="2" t="s">
         <v>16</v>
@@ -1604,26 +1598,26 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="2" t="s">
         <v>19</v>
@@ -1655,26 +1649,26 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="21"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
@@ -1700,36 +1694,36 @@
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="15" t="s">
+      <c r="Y14" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
@@ -1747,26 +1741,26 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="2" t="s">
         <v>27</v>
@@ -1800,26 +1794,26 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="22"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-      <c r="W16" s="23"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="31"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="2" t="s">
         <v>20</v>
@@ -1853,34 +1847,34 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="16" t="s">
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="16" t="s">
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="16" t="s">
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="26"/>
+      <c r="S17" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-      <c r="W17" s="18"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="26"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="2" t="s">
         <v>21</v>
@@ -1914,26 +1908,26 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="21"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="20"/>
-      <c r="U18" s="20"/>
-      <c r="V18" s="20"/>
-      <c r="W18" s="21"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="27"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="29"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="2" t="s">
         <v>22</v>
@@ -1967,26 +1961,26 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="20"/>
-      <c r="U19" s="20"/>
-      <c r="V19" s="20"/>
-      <c r="W19" s="21"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="27"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="29"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="2" t="s">
         <v>23</v>
@@ -2020,26 +2014,26 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="20"/>
-      <c r="U20" s="20"/>
-      <c r="V20" s="20"/>
-      <c r="W20" s="21"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="28"/>
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="29"/>
       <c r="X20" s="1"/>
       <c r="Y20" s="2" t="s">
         <v>14</v>
@@ -2073,26 +2067,26 @@
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="20"/>
-      <c r="U21" s="20"/>
-      <c r="V21" s="20"/>
-      <c r="W21" s="21"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="29"/>
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
@@ -2118,26 +2112,26 @@
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="21"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="21"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="27"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="29"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="13" t="s">
         <v>47</v>
@@ -2165,26 +2159,26 @@
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="21"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="21"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="27"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="29"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="14" t="s">
         <v>48</v>
@@ -2212,26 +2206,26 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="19"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="21"/>
-      <c r="S24" s="19"/>
-      <c r="T24" s="20"/>
-      <c r="U24" s="20"/>
-      <c r="V24" s="20"/>
-      <c r="W24" s="21"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="29"/>
       <c r="X24" s="1"/>
       <c r="Y24" s="14" t="s">
         <v>49</v>
@@ -2259,26 +2253,26 @@
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="19"/>
-      <c r="T25" s="20"/>
-      <c r="U25" s="20"/>
-      <c r="V25" s="20"/>
-      <c r="W25" s="21"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="27"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="29"/>
       <c r="X25" s="1"/>
       <c r="Y25" s="14" t="s">
         <v>50</v>
@@ -2306,26 +2300,26 @@
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="19"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="19"/>
-      <c r="T26" s="20"/>
-      <c r="U26" s="20"/>
-      <c r="V26" s="20"/>
-      <c r="W26" s="21"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="28"/>
+      <c r="V26" s="28"/>
+      <c r="W26" s="29"/>
       <c r="X26" s="1"/>
       <c r="Y26" s="14" t="s">
         <v>51</v>
@@ -2353,26 +2347,26 @@
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="21"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="20"/>
-      <c r="U27" s="20"/>
-      <c r="V27" s="20"/>
-      <c r="W27" s="21"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="27"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="27"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="29"/>
       <c r="X27" s="1"/>
       <c r="Y27" s="13" t="s">
         <v>52</v>
@@ -2400,26 +2394,26 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-      <c r="W28" s="24"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="30"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="32"/>
       <c r="X28" s="1"/>
       <c r="Y28" s="13" t="s">
         <v>53</v>
@@ -2447,30 +2441,30 @@
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
-      <c r="R29" s="35"/>
-      <c r="S29" s="35"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="21"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="29"/>
       <c r="X29" s="1"/>
-      <c r="Y29" s="13" t="s">
+      <c r="Y29" s="14" t="s">
         <v>54</v>
       </c>
       <c r="Z29" s="13"/>
@@ -2496,26 +2490,26 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="21"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="29"/>
       <c r="X30" s="1"/>
       <c r="Y30" s="13" t="s">
         <v>55</v>
@@ -2543,26 +2537,26 @@
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="35"/>
-      <c r="S31" s="35"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="21"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
+      <c r="O31" s="28"/>
+      <c r="P31" s="28"/>
+      <c r="Q31" s="28"/>
+      <c r="R31" s="28"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="28"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="29"/>
       <c r="X31" s="1"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
@@ -2588,26 +2582,26 @@
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="21"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="28"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="29"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="13"/>
       <c r="Z32" s="13"/>
@@ -2633,26 +2627,26 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="21"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="29"/>
       <c r="X33" s="1"/>
       <c r="Y33" s="13"/>
       <c r="Z33" s="13"/>
@@ -2678,26 +2672,26 @@
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="35"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="35"/>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="21"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="28"/>
+      <c r="P34" s="28"/>
+      <c r="Q34" s="28"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+      <c r="W34" s="29"/>
       <c r="X34" s="1"/>
       <c r="Y34" s="13"/>
       <c r="Z34" s="13"/>
@@ -2723,26 +2717,26 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="35"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="35"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
-      <c r="S35" s="35"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
-      <c r="W35" s="21"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
+      <c r="N35" s="28"/>
+      <c r="O35" s="28"/>
+      <c r="P35" s="28"/>
+      <c r="Q35" s="28"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="28"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="29"/>
       <c r="X35" s="1"/>
       <c r="Y35" s="13"/>
       <c r="Z35" s="13"/>
@@ -2768,26 +2762,26 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="35"/>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
-      <c r="O36" s="35"/>
-      <c r="P36" s="35"/>
-      <c r="Q36" s="35"/>
-      <c r="R36" s="35"/>
-      <c r="S36" s="35"/>
-      <c r="T36" s="35"/>
-      <c r="U36" s="35"/>
-      <c r="V36" s="35"/>
-      <c r="W36" s="21"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="28"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
+      <c r="L36" s="28"/>
+      <c r="M36" s="28"/>
+      <c r="N36" s="28"/>
+      <c r="O36" s="28"/>
+      <c r="P36" s="28"/>
+      <c r="Q36" s="28"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="28"/>
+      <c r="T36" s="28"/>
+      <c r="U36" s="28"/>
+      <c r="V36" s="28"/>
+      <c r="W36" s="29"/>
       <c r="X36" s="1"/>
       <c r="Y36" s="13"/>
       <c r="Z36" s="13"/>
@@ -2813,26 +2807,26 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="35"/>
-      <c r="O37" s="35"/>
-      <c r="P37" s="35"/>
-      <c r="Q37" s="35"/>
-      <c r="R37" s="35"/>
-      <c r="S37" s="35"/>
-      <c r="T37" s="35"/>
-      <c r="U37" s="35"/>
-      <c r="V37" s="35"/>
-      <c r="W37" s="21"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="28"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="28"/>
+      <c r="P37" s="28"/>
+      <c r="Q37" s="28"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="28"/>
+      <c r="T37" s="28"/>
+      <c r="U37" s="28"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="29"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="13"/>
       <c r="Z37" s="13"/>
@@ -2858,26 +2852,26 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="35"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
-      <c r="O38" s="35"/>
-      <c r="P38" s="35"/>
-      <c r="Q38" s="35"/>
-      <c r="R38" s="35"/>
-      <c r="S38" s="35"/>
-      <c r="T38" s="35"/>
-      <c r="U38" s="35"/>
-      <c r="V38" s="35"/>
-      <c r="W38" s="21"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="28"/>
+      <c r="P38" s="28"/>
+      <c r="Q38" s="28"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
+      <c r="V38" s="28"/>
+      <c r="W38" s="29"/>
       <c r="X38" s="1"/>
       <c r="Y38" s="13"/>
       <c r="Z38" s="13"/>
@@ -2903,26 +2897,26 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="35"/>
-      <c r="L39" s="35"/>
-      <c r="M39" s="35"/>
-      <c r="N39" s="35"/>
-      <c r="O39" s="35"/>
-      <c r="P39" s="35"/>
-      <c r="Q39" s="35"/>
-      <c r="R39" s="35"/>
-      <c r="S39" s="35"/>
-      <c r="T39" s="35"/>
-      <c r="U39" s="35"/>
-      <c r="V39" s="35"/>
-      <c r="W39" s="21"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="29"/>
       <c r="X39" s="1"/>
       <c r="Y39" s="13"/>
       <c r="Z39" s="13"/>
@@ -2948,26 +2942,26 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="35"/>
-      <c r="L40" s="35"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="35"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="35"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="21"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="28"/>
+      <c r="M40" s="28"/>
+      <c r="N40" s="28"/>
+      <c r="O40" s="28"/>
+      <c r="P40" s="28"/>
+      <c r="Q40" s="28"/>
+      <c r="R40" s="28"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="28"/>
+      <c r="U40" s="28"/>
+      <c r="V40" s="28"/>
+      <c r="W40" s="29"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
@@ -3581,12 +3575,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D5:H16"/>
-    <mergeCell ref="I5:M16"/>
-    <mergeCell ref="D17:H28"/>
-    <mergeCell ref="S5:W7"/>
-    <mergeCell ref="D29:W40"/>
-    <mergeCell ref="I17:M28"/>
     <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="Y14:AE14"/>
     <mergeCell ref="N17:R28"/>
@@ -3594,6 +3582,12 @@
     <mergeCell ref="N5:R7"/>
     <mergeCell ref="N8:R16"/>
     <mergeCell ref="S8:W16"/>
+    <mergeCell ref="D5:H16"/>
+    <mergeCell ref="I5:M16"/>
+    <mergeCell ref="D17:H28"/>
+    <mergeCell ref="S5:W7"/>
+    <mergeCell ref="D29:W40"/>
+    <mergeCell ref="I17:M28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>